<commit_message>
Adjusted image size and added randomizing feature.
</commit_message>
<xml_diff>
--- a/problems.xlsx
+++ b/problems.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\USER\Desktop\ScratchProblems\problemset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linqihuan/Desktop/ScratchProblems/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09957A06-577D-784D-9E08-B17009EF405A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730" tabRatio="274"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="14920" tabRatio="274" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="problems" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="105">
   <si>
     <t>選項B</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -202,90 +203,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Level01_SQ_00005A.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -431,10 +348,6 @@
   </si>
   <si>
     <t>Level01_SQ_00011A.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -537,7 +450,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="12"/>
@@ -878,32 +791,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.25" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
     <col min="3" max="3" width="53" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="28" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.75" style="1" customWidth="1"/>
-    <col min="11" max="11" width="22.375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" style="1" customWidth="1"/>
     <col min="12" max="12" width="23" style="1" customWidth="1"/>
-    <col min="13" max="13" width="5.625" customWidth="1"/>
-    <col min="14" max="14" width="11.625" customWidth="1"/>
-    <col min="15" max="15" width="13.75" style="2" customWidth="1"/>
+    <col min="13" max="13" width="5.6640625" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" ht="16">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -947,12 +860,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" ht="44" customHeight="1">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>18</v>
@@ -973,12 +886,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" ht="16">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>24</v>
@@ -999,12 +912,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="33">
+    <row r="4" spans="1:15" ht="32">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>29</v>
@@ -1022,12 +935,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="33">
+    <row r="5" spans="1:15" ht="32">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>34</v>
@@ -1045,959 +958,289 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="49.5">
+    <row r="6" spans="1:15" ht="48">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="M6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" ht="16">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="M7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="33">
+    <row r="8" spans="1:15" ht="48">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="M8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="49.5">
+    <row r="9" spans="1:15" ht="64">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="M9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="33">
+    <row r="10" spans="1:15" ht="48">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="M10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" ht="32">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="K11" s="1" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="M11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="33">
+    <row r="12" spans="1:15" ht="48">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="M12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" ht="32">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="M13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="33">
+    <row r="14" spans="1:15" ht="32">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="M14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="49.5">
+    <row r="15" spans="1:15" ht="48">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="M15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="33">
+    <row r="16" spans="1:15" ht="32">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="M16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="M17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="M18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="M19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="M20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="M21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="M22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="M23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="M24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="M25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="A26">
-        <v>25</v>
-      </c>
+    <row r="26" spans="3:15">
       <c r="C26"/>
-      <c r="M26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="A27">
-        <v>26</v>
-      </c>
+    </row>
+    <row r="27" spans="3:15">
       <c r="H27" s="3"/>
-      <c r="M27" t="s">
-        <v>102</v>
-      </c>
       <c r="O27" s="4"/>
     </row>
-    <row r="28" spans="1:15">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="M28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="M29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="M30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="M31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="M32" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="M33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="M34" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="M35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="M36" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="M37" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="M38" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="M39" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="M40" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="M41" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="M42" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="M43" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="M44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="M45" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="M46" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="M47" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="M48" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="M49" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13">
-      <c r="A50">
-        <v>49</v>
-      </c>
-      <c r="M50" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13">
-      <c r="A51">
-        <v>50</v>
-      </c>
+    <row r="51" spans="3:3">
       <c r="C51"/>
-      <c r="M51" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13">
-      <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="M52" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13">
-      <c r="A53">
-        <v>52</v>
-      </c>
-      <c r="M53" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13">
-      <c r="A54">
-        <v>53</v>
-      </c>
-      <c r="M54" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="M55" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="M56" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13">
-      <c r="A57">
-        <v>56</v>
-      </c>
-      <c r="M57" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13">
-      <c r="A58">
-        <v>57</v>
-      </c>
-      <c r="M58" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13">
-      <c r="A59">
-        <v>58</v>
-      </c>
-      <c r="M59" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13">
-      <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="M60" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13">
-      <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="M61" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13">
-      <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="M62" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13">
-      <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="M63" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13">
-      <c r="A64">
-        <v>63</v>
-      </c>
-      <c r="M64" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13">
-      <c r="A65">
-        <v>64</v>
-      </c>
-      <c r="M65" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13">
-      <c r="A66">
-        <v>65</v>
-      </c>
-      <c r="M66" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13">
-      <c r="A67">
-        <v>66</v>
-      </c>
-      <c r="M67" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13">
-      <c r="A68">
-        <v>67</v>
-      </c>
-      <c r="M68" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13">
-      <c r="A69">
-        <v>68</v>
-      </c>
-      <c r="M69" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13">
-      <c r="A70">
-        <v>69</v>
-      </c>
-      <c r="M70" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13">
-      <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="M71" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13">
-      <c r="A72">
-        <v>71</v>
-      </c>
-      <c r="M72" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13">
-      <c r="A73">
-        <v>72</v>
-      </c>
-      <c r="M73" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13">
-      <c r="A74">
-        <v>73</v>
-      </c>
-      <c r="M74" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13">
-      <c r="A75">
-        <v>74</v>
-      </c>
-      <c r="M75" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13">
-      <c r="A76">
-        <v>75</v>
-      </c>
+    </row>
+    <row r="76" spans="3:3">
       <c r="C76"/>
-      <c r="M76" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13">
-      <c r="A77">
-        <v>76</v>
-      </c>
-      <c r="M77" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="M78" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13">
-      <c r="A79">
-        <v>78</v>
-      </c>
-      <c r="M79" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13">
-      <c r="A80">
-        <v>79</v>
-      </c>
-      <c r="M80" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13">
-      <c r="A81">
-        <v>80</v>
-      </c>
-      <c r="M81" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13">
-      <c r="A82">
-        <v>81</v>
-      </c>
-      <c r="M82" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13">
-      <c r="A83">
-        <v>82</v>
-      </c>
-      <c r="M83" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13">
-      <c r="A84">
-        <v>83</v>
-      </c>
-      <c r="M84" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13">
-      <c r="A85">
-        <v>84</v>
-      </c>
-      <c r="M85" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13">
-      <c r="A86">
-        <v>85</v>
-      </c>
-      <c r="M86" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13">
-      <c r="A87">
-        <v>86</v>
-      </c>
-      <c r="M87" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13">
-      <c r="A88">
-        <v>87</v>
-      </c>
-      <c r="M88" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13">
-      <c r="A89">
-        <v>88</v>
-      </c>
-      <c r="M89" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13">
-      <c r="A90">
-        <v>89</v>
-      </c>
-      <c r="M90" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13">
-      <c r="A91">
-        <v>90</v>
-      </c>
-      <c r="M91" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13">
-      <c r="A92">
-        <v>91</v>
-      </c>
-      <c r="M92" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13">
-      <c r="A93">
-        <v>92</v>
-      </c>
-      <c r="M93" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13">
-      <c r="A94">
-        <v>93</v>
-      </c>
-      <c r="M94" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13">
-      <c r="A95">
-        <v>94</v>
-      </c>
-      <c r="M95" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13">
-      <c r="A96">
-        <v>95</v>
-      </c>
-      <c r="M96" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13">
-      <c r="A97">
-        <v>96</v>
-      </c>
-      <c r="M97" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="98" spans="1:13">
-      <c r="A98">
-        <v>97</v>
-      </c>
-      <c r="M98" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13">
-      <c r="A99">
-        <v>98</v>
-      </c>
-      <c r="M99" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="100" spans="1:13">
-      <c r="A100">
-        <v>99</v>
-      </c>
-      <c r="M100" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13">
-      <c r="A101">
-        <v>100</v>
-      </c>
+    </row>
+    <row r="101" spans="3:3">
       <c r="C101"/>
-      <c r="M101" t="s">
-        <v>44</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Fixed display problems when both text and image are present in a choice
</commit_message>
<xml_diff>
--- a/problems.xlsx
+++ b/problems.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/linqihuan/Desktop/ScratchProblems/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\USER\Desktop\ScratchProblems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09957A06-577D-784D-9E08-B17009EF405A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="14920" tabRatio="274" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="14925" tabRatio="274"/>
   </bookViews>
   <sheets>
     <sheet name="problems" sheetId="1" r:id="rId1"/>
@@ -371,10 +370,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>假如今天我想讓角色在遊戲一開始，出現在螢幕的正中間，請問我會使用到下列哪一個積木呢？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Level01_SQ_00013D.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -419,18 +414,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>假如今天小鹿改變了角色的方向，卻發現畫面中的角色沒有朝向它應該面對的方向。請問小鹿該使用下列哪一個積木來解決這個問題呢？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>假如我想設計一個遊戲，其中有一個功能是擲骰子，按照骰子的點數來決定角色的移動步數，請問我會用到下列哪一個積木呢？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>假如我想設計一個吹氣球的遊戲，其中的氣球會隨著時間長得越來越大，我該使用下列哪一個積木，讓氣球變大呢？</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Level01_SQ_00015C.png</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -444,13 +427,29 @@
   </si>
   <si>
     <t>Level01_SQ_00015A.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>假如我想設計一個遊戲功能叫擲骰子，如果我想要擲一次骰子並顯示點數，請問我會用到下列哪一個積木呢？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>假如今天小鹿改變了角色的方向角度，卻發現畫面中的角色沒有朝向它應該面對的角度。請問小鹿該使用下列哪一個積木來解決這個問題呢？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>假如我想設計一個吹氣球的遊戲，其中的氣球角色需要變大。我該使用下列哪一個積木來做到這件事情呢？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>假如今天我想讓角色在遊戲一開始，定位到螢幕的正中間，請問我會使用到下列哪一個積木呢？</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3">
     <font>
       <sz val="12"/>
@@ -791,32 +790,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.125" customWidth="1"/>
     <col min="3" max="3" width="53" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.125" style="1" customWidth="1"/>
     <col min="7" max="7" width="28" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22.375" style="1" customWidth="1"/>
     <col min="12" max="12" width="23" style="1" customWidth="1"/>
-    <col min="13" max="13" width="5.6640625" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="5.625" customWidth="1"/>
+    <col min="14" max="14" width="11.625" customWidth="1"/>
+    <col min="15" max="15" width="13.625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16">
+    <row r="1" spans="1:15">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -860,7 +859,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="44" customHeight="1">
+    <row r="2" spans="1:15" ht="44.1" customHeight="1">
       <c r="A2">
         <v>1</v>
       </c>
@@ -886,7 +885,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="16">
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -912,12 +911,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="32">
+    <row r="4" spans="1:15" ht="33">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>29</v>
@@ -935,12 +934,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="32">
+    <row r="5" spans="1:15" ht="33">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>34</v>
@@ -958,7 +957,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="48">
+    <row r="6" spans="1:15" ht="49.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -981,7 +980,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="16">
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1007,7 +1006,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="48">
+    <row r="8" spans="1:15" ht="49.5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1033,7 +1032,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="64">
+    <row r="9" spans="1:15" ht="66">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1059,7 +1058,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="48">
+    <row r="10" spans="1:15" ht="49.5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1082,7 +1081,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="32">
+    <row r="11" spans="1:15" ht="33">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1108,12 +1107,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="48">
+    <row r="12" spans="1:15" ht="33">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>80</v>
@@ -1122,7 +1121,7 @@
         <v>78</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>79</v>
@@ -1131,7 +1130,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="32">
+    <row r="13" spans="1:15" ht="33">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1157,70 +1156,70 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="32">
+    <row r="14" spans="1:15" ht="33">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="48">
+    <row r="15" spans="1:15" ht="49.5">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="M15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="32">
+    <row r="16" spans="1:15" ht="33">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="M16" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Added random and direct problem selection functionality
</commit_message>
<xml_diff>
--- a/problems.xlsx
+++ b/problems.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr hidePivotFieldList="1"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\USER\Desktop\ScratchProblems\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Coding_curriculum_SVN\其他\03. Tools\題庫隨機測驗app\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="218">
   <si>
     <t>選項B</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -444,13 +444,373 @@
   <si>
     <t>假如今天我想讓角色在遊戲一開始，定位到螢幕的正中間，請問我會使用到下列哪一個積木呢？</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>關於此積木的敘述，以下何者正確 ? (  )</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00101.png</t>
+  </si>
+  <si>
+    <t>x移動10</t>
+  </si>
+  <si>
+    <t>y移動10</t>
+  </si>
+  <si>
+    <t>根據方向移動10</t>
+  </si>
+  <si>
+    <t>以上皆錯誤</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>以下何種積木組合不是移動100 ? (  )</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00102A.png</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00102B.png</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00102C.png</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00102D.png</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>根據此圖，現在方向(Direction)為90，且移動(move)100，兔
+子將會往哪個方向移動 ? (  )</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00103.png</t>
+  </si>
+  <si>
+    <t>向左</t>
+  </si>
+  <si>
+    <t>向右</t>
+  </si>
+  <si>
+    <t>向上</t>
+  </si>
+  <si>
+    <t>向下</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>根據此圖，現在方向(Direction)為90，以下何圖呈現
+方向(Direction)為-90 ? (  )</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00104.png</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00104A.png</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00104B.png</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00104C.png</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00104D.png</t>
+  </si>
+  <si>
+    <t>執行此積木後，角色將會有什麼反應? ( )</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00105.png</t>
+  </si>
+  <si>
+    <t>角色將會定點到 x : 0 y : 0的位置</t>
+  </si>
+  <si>
+    <t>角色將會以隨機的速度
+移動到 x : 0 y : 0的位置</t>
+  </si>
+  <si>
+    <t>角色將會定點隨機的位置</t>
+  </si>
+  <si>
+    <t>角色將會以隨機的速度
+移動到隨機的位置</t>
+  </si>
+  <si>
+    <t>以下何種積木組合可以達到角色一直隨著滑鼠移動 ?（）</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00106A.png</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00106B.png</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00106C.png</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00106D.png</t>
+  </si>
+  <si>
+    <t>關於執行此積木的敘述，以下何者選項正確 ? (  )</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00107.png</t>
+  </si>
+  <si>
+    <t>1秒後，角色將會滑行到x:50 y:50</t>
+  </si>
+  <si>
+    <t>滑行到x:50 y:50的時間要根據角色的
+速度而定</t>
+  </si>
+  <si>
+    <t>角色在還沒開始執行此積木時位置一定
+為x:0 y:0</t>
+  </si>
+  <si>
+    <t>以上皆正確</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>根據下圖，x:40 y:80，角色將會在哪一個區塊 ? ( )</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00108.png</t>
+  </si>
+  <si>
+    <t>根據下圖，x:-50 y:100，角色將會在哪一個區塊 ? ( )</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00109.png</t>
+  </si>
+  <si>
+    <t>關於此積木的敘述，以下何者正確? (  )</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00110.png</t>
+  </si>
+  <si>
+    <t>此積木的涵義為鼠標的方向</t>
+  </si>
+  <si>
+    <t>在"mouse pointer"這個方框內可以
+放入任何積木</t>
+  </si>
+  <si>
+    <t>在"mouse pointer"這個方框內無法
+放入任何積木</t>
+  </si>
+  <si>
+    <t>在"mouse pointer"這個方框內只能
+放入同為陀圓形狀積木</t>
+  </si>
+  <si>
+    <t>以下何者最終位置不一定會在x : 100 y : 0 ? (  )</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00111A.png</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00111B.png</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00111C.png</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00111D.png</t>
+  </si>
+  <si>
+    <t>關於此積木的敘述，以下何者錯誤? (  )</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00112.png</t>
+  </si>
+  <si>
+    <t>此積木可以在motion code 找到</t>
+  </si>
+  <si>
+    <t>邊緣指的是舞台的邊緣</t>
+  </si>
+  <si>
+    <t>此積木可以使角色移動到邊緣</t>
+  </si>
+  <si>
+    <t>此積木可以使角色不跑出邊緣</t>
+  </si>
+  <si>
+    <t>迴轉方式左右</t>
+  </si>
+  <si>
+    <t>此積木可以在looks code 找到</t>
+  </si>
+  <si>
+    <t>此左右的方向為鏡像</t>
+  </si>
+  <si>
+    <t>此左右的方向為direction +90度</t>
+  </si>
+  <si>
+    <t>此左右的方向為direction +180度</t>
+  </si>
+  <si>
+    <t>此積木可以放入積木move ( )的空格里</t>
+  </si>
+  <si>
+    <t>按下左方空格後將會在舞台裡顯示目
+前此costume的x座標</t>
+  </si>
+  <si>
+    <t>x position可以放入任何含有框框的積木</t>
+  </si>
+  <si>
+    <t>x position只能放入含有同為橢圓形框框的
+積木</t>
+  </si>
+  <si>
+    <t>前後兩個框框都可以自己做更改</t>
+  </si>
+  <si>
+    <t>根據此圖，角色將持續說出"hello"兩秒</t>
+  </si>
+  <si>
+    <t>根據此圖，角色在兩秒後將不會說出任何話</t>
+  </si>
+  <si>
+    <t>造型換mm</t>
+  </si>
+  <si>
+    <t>此框框內為該角色的costume名稱</t>
+  </si>
+  <si>
+    <t>此框框內為該角色的costume編號</t>
+  </si>
+  <si>
+    <t>此積木可以在control code 找到</t>
+  </si>
+  <si>
+    <t>關於執行此積木的敘述，以下何者完全正確? (  )</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>將會變成當前編號下一個的背景
+假設現在標號為1，執行此積木後將會
+變成編號為2的背景</t>
+  </si>
+  <si>
+    <t>將會變成當前名稱下一個的背景
+變成名稱為2的背景</t>
+  </si>
+  <si>
+    <t>不管在任何情況下，執行此積木後將會隨機
+更換背景</t>
+  </si>
+  <si>
+    <t>執行此積木後背景將會動起來</t>
+  </si>
+  <si>
+    <t>設初始seize為100，執行此積木後，seize將變為多少? (  )</t>
+  </si>
+  <si>
+    <t>Change seize</t>
+  </si>
+  <si>
+    <t>設初始seize為100，執行此積木兩次後，seize將變為多少? (  )</t>
+  </si>
+  <si>
+    <t>設定為80趴</t>
+  </si>
+  <si>
+    <t>關於此積木表示的涵義為何 ? (  )</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00120.png</t>
+  </si>
+  <si>
+    <t>一個數值，隨機的數字</t>
+  </si>
+  <si>
+    <t>一個數值，隨著角色目前所在
+舞台的 y位置變化</t>
+  </si>
+  <si>
+    <t>是固定的數值，角色初始位置</t>
+  </si>
+  <si>
+    <t>是固定的數值，角色初始位置，能夠做
+填寫的數</t>
+  </si>
+  <si>
+    <t>此圖為costume原圖，試問當發生下列相對應的圖像效果，
+何者錯誤 ? (  )</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00121.png</t>
+  </si>
+  <si>
+    <t>魚眼</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00121A.png</t>
+  </si>
+  <si>
+    <t>旋轉</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00121B.png</t>
+  </si>
+  <si>
+    <t>幻影</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00121C.png</t>
+  </si>
+  <si>
+    <t>馬賽克</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00121D.png</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00122.png</t>
+  </si>
+  <si>
+    <t>此積木被執行後可將角色(sprite)隱藏</t>
+  </si>
+  <si>
+    <t>在隱藏後，角色人仍然可以做出有
+些積木給的指令像是move steps</t>
+  </si>
+  <si>
+    <t>此積木被執行後，將無法利用別的積木使角
+色顯示</t>
+  </si>
+  <si>
+    <t>如果使用ghost effect設為100，
+看起來效果將會與hide一樣</t>
+  </si>
+  <si>
+    <t>Level01_SQ_00123.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -472,13 +832,41 @@
       <name val="PMingLiu"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -490,12 +878,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -511,9 +900,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="一般 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -793,8 +1195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5"/>
@@ -1225,12 +1627,674 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="3:15">
-      <c r="C26"/>
-    </row>
-    <row r="27" spans="3:15">
-      <c r="H27" s="3"/>
+    <row r="17" spans="1:15">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="J19" s="8"/>
+      <c r="K19" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="J21" s="5"/>
+      <c r="K21" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="I22" s="6"/>
+      <c r="J22" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="K22" s="6"/>
+      <c r="L22" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="I24" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="J24" s="8"/>
+      <c r="K24" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="H26" s="5"/>
+      <c r="I26" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="J26" s="5"/>
+      <c r="K26" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="M27" s="5"/>
       <c r="O27" s="4"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="J30" s="5"/>
+      <c r="K30" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="L33" s="7"/>
+      <c r="M33" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E34" s="5">
+        <v>10</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5">
+        <v>90</v>
+      </c>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5">
+        <v>100</v>
+      </c>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5">
+        <v>110</v>
+      </c>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E35" s="5">
+        <v>0</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5">
+        <v>64</v>
+      </c>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5">
+        <v>80</v>
+      </c>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5">
+        <v>180</v>
+      </c>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="L37" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="M37" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
     </row>
     <row r="51" spans="3:3">
       <c r="C51"/>

</xml_diff>